<commit_message>
Updated script to handle different environments along with batch processing logic to overcome SDK limitations.
</commit_message>
<xml_diff>
--- a/Boto3/aws_user_audit/files/AWS_User_Audit_2025_05_28.xlsx
+++ b/Boto3/aws_user_audit/files/AWS_User_Audit_2025_05_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +451,11 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>State</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Users</t>
         </is>
       </c>
@@ -458,14 +463,10 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>i-00422ea8bc1d8ae66</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>test-ec2-1</t>
-        </is>
-      </c>
+          <t>i-056820ee844baf41e</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
           <t>Linux/UNIX</t>
@@ -473,21 +474,27 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Hello, World!</t>
+          <t>running</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">root
+dhcpcd
+tss
+pollinate
+ubuntu
+</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>i-03715bb3fd6ee5769</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>test-ec2-2</t>
-        </is>
-      </c>
+          <t>i-0c4995636b4a3f8ad</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
           <t>Linux/UNIX</t>
@@ -495,21 +502,27 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Hello, World!</t>
+          <t>running</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">root
+dhcpcd
+tss
+pollinate
+ubuntu
+</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>i-047f2eb739b976d10</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>test-ec2-3</t>
-        </is>
-      </c>
+          <t>i-046e18bd3080b03ce</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
           <t>Linux/UNIX</t>
@@ -517,7 +530,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Hello, World!</t>
+          <t>running</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">root
+dhcpcd
+tss
+pollinate
+ubuntu
+</t>
         </is>
       </c>
     </row>

</xml_diff>